<commit_message>
vary latency and rerun, rename availability
</commit_message>
<xml_diff>
--- a/out/models/0-combined.xlsx
+++ b/out/models/0-combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\research\coupling-quartermaster\out\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C31A48-D0B9-432F-9405-45A10BFCF29D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1920345-C107-4BC2-9A58-0CE340B6F321}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A-100-Naive-VaryLoad" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="ExternalData_2" localSheetId="1" hidden="1">'C-100-LoadShedding-VaryLoad'!$A$1:$AB$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24860,7 +24861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787EE20C-5506-4B23-A068-802EDFD0097D}">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -42314,7 +42315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>

</xml_diff>